<commit_message>
update MS-OXCMSG RSaccording to comments
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCMSG/MS-OXCMSG_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCMSG/MS-OXCMSG_RequirementSpecification.xlsx
@@ -8910,9 +8910,6 @@
     <t>[In Appendix A: Product Behavior] &lt;21&gt; Section 3.2.5.2:  Implementation does initialize the following properties:PidTagDisplayBcc ([MS-OXOMSG] section 2.2.1.7), PidTagDisplayCc ([MS-OXOMSG] section 2.2.1.8) and PidTagDisplayTo ([MS-OXOMSG] section 2.2.1.9). (Exchange 2010 and Exchange 2013 followin this behavior.)</t>
   </si>
   <si>
-    <t>[In Appendix A: Product Behavior] &lt;21&gt; Section 3.2.5.2: Exchange 2016 and Exchange 2019 Preview do not initialize the following properties: PidTagDisplayBcc ([MS-OXOMSG] section 2.2.1.7), PidTagDisplayCc ([MS-OXOMSG] section 2.2.1.8) and PidTagDisplayTo ([MS-OXOMSG] section 2.2.1.9). (Exchange 2016 and above follow this behavior.)</t>
-  </si>
-  <si>
     <t>MS-OXCMSG_R164101</t>
   </si>
   <si>
@@ -8929,6 +8926,9 @@
   </si>
   <si>
     <t>[In Property Value Types] PtypObject or PtypEmbeddedTable (PT_OBJECT) is  that  the property value is a Component Object Model (COM) object, as specified in section 2.11.1.5. with Property Type Value 0x000D,%x0D.00.</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] &lt;21&gt; Section 3.2.5.2: Implementation does not initialize the following properties: PidTagDisplayBcc ([MS-OXOMSG] section 2.2.1.7), PidTagDisplayCc ([MS-OXOMSG] section 2.2.1.8) and PidTagDisplayTo ([MS-OXOMSG] section 2.2.1.9). (Exchange 2016 and above follow this behavior.)</t>
   </si>
 </sst>
 </file>
@@ -9200,21 +9200,6 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -9239,115 +9224,26 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="39">
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -9686,6 +9582,110 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -9815,34 +9815,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I1254" tableType="xml" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37" connectionId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I1254" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
   <autoFilter ref="A19:I1254"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="36">
+    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="35">
+    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="34">
+    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="33">
+    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="32">
+    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="31">
+    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="30">
+    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="29">
+    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="28">
+    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -9851,12 +9851,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26" tableBorderDxfId="24" totalsRowBorderDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A12:C15"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Scope" dataDxfId="22"/>
-    <tableColumn id="2" name="Test" dataDxfId="21"/>
-    <tableColumn id="3" name="Description" dataDxfId="20"/>
+    <tableColumn id="1" name="Scope" dataDxfId="2"/>
+    <tableColumn id="2" name="Test" dataDxfId="1"/>
+    <tableColumn id="3" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -10152,9 +10152,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L1256"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1251" sqref="C1251"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -10208,127 +10206,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -10341,12 +10339,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -10359,12 +10357,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -10377,12 +10375,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -10395,60 +10393,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="41"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="45"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -23228,13 +23226,13 @@
         <v>19</v>
       </c>
       <c r="F525" s="29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G525" s="29" t="s">
         <v>15</v>
       </c>
       <c r="H525" s="29" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I525" s="31"/>
     </row>
@@ -23278,13 +23276,13 @@
         <v>19</v>
       </c>
       <c r="F527" s="29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G527" s="29" t="s">
         <v>15</v>
       </c>
       <c r="H527" s="29" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I527" s="31"/>
     </row>
@@ -23328,13 +23326,13 @@
         <v>19</v>
       </c>
       <c r="F529" s="29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G529" s="29" t="s">
         <v>15</v>
       </c>
       <c r="H529" s="29" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I529" s="31"/>
     </row>
@@ -23478,13 +23476,13 @@
         <v>19</v>
       </c>
       <c r="F535" s="29" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G535" s="29" t="s">
         <v>15</v>
       </c>
       <c r="H535" s="29" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I535" s="31"/>
     </row>
@@ -23528,13 +23526,13 @@
         <v>19</v>
       </c>
       <c r="F537" s="29" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G537" s="29" t="s">
         <v>15</v>
       </c>
       <c r="H537" s="29" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I537" s="31"/>
     </row>
@@ -34683,7 +34681,7 @@
         <v>17</v>
       </c>
       <c r="I977" s="31" t="s">
-        <v>2887</v>
+        <v>2886</v>
       </c>
     </row>
     <row r="978" spans="1:9" ht="30">
@@ -39613,13 +39611,13 @@
     </row>
     <row r="1167" spans="1:9" ht="60">
       <c r="A1167" s="29" t="s">
-        <v>2885</v>
+        <v>2884</v>
       </c>
       <c r="B1167" s="30" t="s">
         <v>1236</v>
       </c>
       <c r="C1167" s="31" t="s">
-        <v>2884</v>
+        <v>2890</v>
       </c>
       <c r="D1167" s="22" t="s">
         <v>2522</v>
@@ -39640,7 +39638,7 @@
     </row>
     <row r="1168" spans="1:9" ht="60">
       <c r="A1168" s="29" t="s">
-        <v>2886</v>
+        <v>2885</v>
       </c>
       <c r="B1168" s="30" t="s">
         <v>1236</v>
@@ -39934,7 +39932,7 @@
         <v>1236</v>
       </c>
       <c r="C1178" s="20" t="s">
-        <v>2888</v>
+        <v>2887</v>
       </c>
       <c r="D1178" s="22" t="s">
         <v>2690</v>
@@ -40584,7 +40582,7 @@
         <v>1236</v>
       </c>
       <c r="C1202" s="31" t="s">
-        <v>2889</v>
+        <v>2888</v>
       </c>
       <c r="D1202" s="29"/>
       <c r="E1202" s="29" t="s">
@@ -41835,7 +41833,7 @@
         <v>1457</v>
       </c>
       <c r="C1251" s="31" t="s">
-        <v>2890</v>
+        <v>2889</v>
       </c>
       <c r="D1251" s="29"/>
       <c r="E1251" s="29" t="s">
@@ -41937,6 +41935,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -41944,84 +41947,79 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A636:H636 A20:I31 A32:H32 A33:I635 A637:I1254">
-    <cfRule type="expression" dxfId="19" priority="65">
+    <cfRule type="expression" dxfId="38" priority="65">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="66">
+    <cfRule type="expression" dxfId="37" priority="66">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="73">
+    <cfRule type="expression" dxfId="36" priority="73">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A636:H636 A20:I31 A32:H32 A33:I635 A637:I1254">
-    <cfRule type="expression" dxfId="16" priority="19">
+    <cfRule type="expression" dxfId="35" priority="19">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="20">
+    <cfRule type="expression" dxfId="34" priority="20">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="21">
+    <cfRule type="expression" dxfId="33" priority="21">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:F1254">
-    <cfRule type="expression" dxfId="13" priority="25">
+    <cfRule type="expression" dxfId="32" priority="25">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="26">
+    <cfRule type="expression" dxfId="31" priority="26">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I636">
-    <cfRule type="expression" dxfId="11" priority="10">
+    <cfRule type="expression" dxfId="30" priority="10">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="11">
+    <cfRule type="expression" dxfId="29" priority="11">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="12">
+    <cfRule type="expression" dxfId="28" priority="12">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I636">
-    <cfRule type="expression" dxfId="8" priority="7">
+    <cfRule type="expression" dxfId="27" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="26" priority="8">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="9">
+    <cfRule type="expression" dxfId="25" priority="9">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I32">
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="24" priority="4">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="23" priority="5">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="6">
+    <cfRule type="expression" dxfId="22" priority="6">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I32">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="21" priority="1">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="20" priority="2">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="19" priority="3">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -42059,6 +42057,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -42107,32 +42120,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -42152,9 +42143,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[MS-OXCMSG]: Update capture code according to new release RS
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCMSG/MS-OXCMSG_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCMSG/MS-OXCMSG_RequirementSpecification.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6716CCC-B423-418C-9A65-C086EF7E8307}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570"/>
+    <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -20,8 +21,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="tmp579F" type="4" refreshedVersion="0" background="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="tmp579F" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\v-xinwli\AppData\Local\Temp\tmp579F.tmp" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
@@ -8949,7 +8950,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="0.0.0"/>
@@ -9215,21 +9216,6 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -9254,115 +9240,26 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="39">
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -9701,6 +9598,110 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -9830,34 +9831,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I1256" tableType="xml" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37" connectionId="1">
-  <autoFilter ref="A19:I1256"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I1256" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
+  <autoFilter ref="A19:I1256" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="36">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="35">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="34">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="ns1:Description" name="Description" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="33">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="32">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="31">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="30">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="29">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="28">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -9866,12 +9867,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26" tableBorderDxfId="24" totalsRowBorderDxfId="23">
-  <autoFilter ref="A12:C15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+  <autoFilter ref="A12:C15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Scope" dataDxfId="22"/>
-    <tableColumn id="2" name="Test" dataDxfId="21"/>
-    <tableColumn id="3" name="Description" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Scope" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9953,6 +9954,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -9988,6 +10006,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -10163,13 +10198,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L1258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1178" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1180" sqref="C1180"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -10223,127 +10256,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -10356,12 +10389,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -10374,12 +10407,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -10392,12 +10425,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -10410,60 +10443,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="41"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="45"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -20602,7 +20635,7 @@
         <v>15</v>
       </c>
       <c r="H420" s="29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I420" s="31"/>
     </row>
@@ -42002,6 +42035,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -42009,102 +42047,97 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A638:H638 A20:I31 A32:H32 A639:I1256 A33:I637">
-    <cfRule type="expression" dxfId="19" priority="65">
+    <cfRule type="expression" dxfId="38" priority="65">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="66">
+    <cfRule type="expression" dxfId="37" priority="66">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="73">
+    <cfRule type="expression" dxfId="36" priority="73">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A638:H638 A20:I31 A32:H32 A639:I1256 A33:I637">
-    <cfRule type="expression" dxfId="16" priority="19">
+    <cfRule type="expression" dxfId="35" priority="19">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="20">
+    <cfRule type="expression" dxfId="34" priority="20">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="21">
+    <cfRule type="expression" dxfId="33" priority="21">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:F1256">
-    <cfRule type="expression" dxfId="13" priority="25">
+    <cfRule type="expression" dxfId="32" priority="25">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="26">
+    <cfRule type="expression" dxfId="31" priority="26">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I638">
-    <cfRule type="expression" dxfId="11" priority="10">
+    <cfRule type="expression" dxfId="30" priority="10">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="11">
+    <cfRule type="expression" dxfId="29" priority="11">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="12">
+    <cfRule type="expression" dxfId="28" priority="12">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I638">
-    <cfRule type="expression" dxfId="8" priority="7">
+    <cfRule type="expression" dxfId="27" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="26" priority="8">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="9">
+    <cfRule type="expression" dxfId="25" priority="9">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I32">
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="24" priority="4">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="23" priority="5">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="6">
+    <cfRule type="expression" dxfId="22" priority="6">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I32">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="21" priority="1">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="20" priority="2">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="19" priority="3">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F1256">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F1256" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$A$13:$A$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E1256">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E1256" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Protocol,Product"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G1256">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G1256" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Informative,Normative"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"In, Out"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H1256">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H1256" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"Non-testable, Unverified, Adapter, Test Case"</formula1>
     </dataValidation>
   </dataValidations>
@@ -42124,18 +42157,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -42188,6 +42221,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -42197,14 +42238,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Update RS according to v20190618 document.
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCMSG/MS-OXCMSG_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCMSG/MS-OXCMSG_RequirementSpecification.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{378B43EC-BBE2-44CD-9FF1-CD29B0DA9A36}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47EA9322-68BC-40B5-8D8F-2A69ABA24C98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -8347,9 +8347,6 @@
     <t>Verified by derived requirement: MS-OXCMSG_R3004.</t>
   </si>
   <si>
-    <t>MS-OXCMSG_R3021</t>
-  </si>
-  <si>
     <t>MS-OXCMSG_R1674:i</t>
   </si>
   <si>
@@ -8401,9 +8398,6 @@
     <t>MS-OXCMSG_R1826:i</t>
   </si>
   <si>
-    <t>[In Appendix A: Product Behavior] [PartialCompletion] A nonzero value indicates the server was unable to modify one or more of the Message objects represented in the MessageIds field. (Exchange 2007 and exchange 2016 follow this behavior.)</t>
-  </si>
-  <si>
     <t>[In Appendix A: Product Behavior] Implementation does initialize the properties: PidTagCreatorName, PidTagCreatorEntryId, PidTagLastModifierName, PidTagLastModifierEntryId, PidTagLastModificationTime, PidTagMessageLocaleId  and PidTagLocaleId. (Exchange 2007 and Exchange 2010 follow this behavior.)</t>
   </si>
   <si>
@@ -8558,9 +8552,6 @@
   </si>
   <si>
     <t>2.2.2.29</t>
-  </si>
-  <si>
-    <t>[In Appendix A: Product Behavior] &lt;21&gt; Section 3.2.5.2:  Implementation does initialize the following properties:PidTagDisplayBcc ([MS-OXOMSG] section 2.2.1.7), PidTagDisplayCc ([MS-OXOMSG] section 2.2.1.8) and PidTagDisplayTo ([MS-OXOMSG] section 2.2.1.9). (Exchange 2010 and Exchange 2013 followin this behavior.)</t>
   </si>
   <si>
     <t>MS-OXCMSG_R164101</t>
@@ -9033,6 +9024,18 @@
   </si>
   <si>
     <t>[In Appendix A: Product Behavior] &lt;21&gt; Section 3.2.5.2: Implementation does not initialize the following properties: PidTagCreatorName ([MS-OXPROPS] section 2.656), PidTagCreatorEntryId (section 2.2.1.31), PidTagLastModifierName ([MS-OXCPRPT] section 2.2.1.5), PidTagLastModifierEntryId (section 2.2.1.32), PidTagLastModificationTime (section 2.2.2.2), PidTagMessageLocaleId (section 2.2.1.5) and PidTagLocaleId ([MS-OXPROPS] section 2.770). (Exchange 2013 follows this behavior.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] &lt;21&gt; Section 3.2.5.2:  Implementation does initialize the following properties:PidTagDisplayBcc ([MS-OXOMSG] section 2.2.1.7), PidTagDisplayCc ([MS-OXOMSG] section 2.2.1.8) and PidTagDisplayTo ([MS-OXOMSG] section 2.2.1.9). (Exchange 2010 and Exchange 2013 follow this behavior.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MS-OXCMSG_R3021</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] [PartialCompletion] A nonzero value indicates the server was unable to modify one or more of the Message objects represented in the MessageIds field. (Exchange 2007 follows this behavior.)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -9347,7 +9350,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="39">
     <dxf>
@@ -9969,7 +9972,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -10292,7 +10295,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L1258"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A1158" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1162" sqref="C1162"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10335,7 +10340,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>2807</v>
+        <v>2804</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>26</v>
@@ -10944,7 +10949,7 @@
         <v>17</v>
       </c>
       <c r="I32" s="24" t="s">
-        <v>2716</v>
+        <v>2714</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -11302,7 +11307,7 @@
         <v>1234</v>
       </c>
       <c r="C46" s="20" t="s">
-        <v>2808</v>
+        <v>2805</v>
       </c>
       <c r="D46" s="29"/>
       <c r="E46" s="29" t="s">
@@ -11377,7 +11382,7 @@
         <v>1234</v>
       </c>
       <c r="C49" s="20" t="s">
-        <v>2810</v>
+        <v>2807</v>
       </c>
       <c r="D49" s="29"/>
       <c r="E49" s="29" t="s">
@@ -11427,7 +11432,7 @@
         <v>1235</v>
       </c>
       <c r="C51" s="20" t="s">
-        <v>2811</v>
+        <v>2808</v>
       </c>
       <c r="D51" s="29"/>
       <c r="E51" s="29" t="s">
@@ -11704,7 +11709,7 @@
         <v>1237</v>
       </c>
       <c r="C62" s="20" t="s">
-        <v>2812</v>
+        <v>2809</v>
       </c>
       <c r="D62" s="29"/>
       <c r="E62" s="29" t="s">
@@ -11854,7 +11859,7 @@
         <v>1239</v>
       </c>
       <c r="C68" s="20" t="s">
-        <v>2813</v>
+        <v>2810</v>
       </c>
       <c r="D68" s="29"/>
       <c r="E68" s="29" t="s">
@@ -12887,7 +12892,7 @@
         <v>1242</v>
       </c>
       <c r="C109" s="20" t="s">
-        <v>2814</v>
+        <v>2811</v>
       </c>
       <c r="D109" s="29"/>
       <c r="E109" s="29" t="s">
@@ -13012,7 +13017,7 @@
         <v>1243</v>
       </c>
       <c r="C114" s="20" t="s">
-        <v>2815</v>
+        <v>2812</v>
       </c>
       <c r="D114" s="29"/>
       <c r="E114" s="29" t="s">
@@ -13137,7 +13142,7 @@
         <v>1244</v>
       </c>
       <c r="C119" s="20" t="s">
-        <v>2816</v>
+        <v>2813</v>
       </c>
       <c r="D119" s="29"/>
       <c r="E119" s="29" t="s">
@@ -13289,7 +13294,7 @@
         <v>1245</v>
       </c>
       <c r="C125" s="20" t="s">
-        <v>2817</v>
+        <v>2814</v>
       </c>
       <c r="D125" s="29"/>
       <c r="E125" s="29" t="s">
@@ -13441,7 +13446,7 @@
         <v>1246</v>
       </c>
       <c r="C131" s="20" t="s">
-        <v>2818</v>
+        <v>2815</v>
       </c>
       <c r="D131" s="29"/>
       <c r="E131" s="29" t="s">
@@ -13618,7 +13623,7 @@
         <v>1247</v>
       </c>
       <c r="C138" s="31" t="s">
-        <v>2773</v>
+        <v>2770</v>
       </c>
       <c r="D138" s="29"/>
       <c r="E138" s="29" t="s">
@@ -13693,7 +13698,7 @@
         <v>1248</v>
       </c>
       <c r="C141" s="31" t="s">
-        <v>2774</v>
+        <v>2771</v>
       </c>
       <c r="D141" s="29"/>
       <c r="E141" s="29" t="s">
@@ -13743,7 +13748,7 @@
         <v>1249</v>
       </c>
       <c r="C143" s="31" t="s">
-        <v>2775</v>
+        <v>2772</v>
       </c>
       <c r="D143" s="29"/>
       <c r="E143" s="29" t="s">
@@ -14470,7 +14475,7 @@
         <v>1250</v>
       </c>
       <c r="C172" s="20" t="s">
-        <v>2819</v>
+        <v>2816</v>
       </c>
       <c r="D172" s="29"/>
       <c r="E172" s="29" t="s">
@@ -14545,7 +14550,7 @@
         <v>1251</v>
       </c>
       <c r="C175" s="31" t="s">
-        <v>2776</v>
+        <v>2773</v>
       </c>
       <c r="D175" s="29"/>
       <c r="E175" s="29" t="s">
@@ -14645,7 +14650,7 @@
         <v>1252</v>
       </c>
       <c r="C179" s="31" t="s">
-        <v>2777</v>
+        <v>2774</v>
       </c>
       <c r="D179" s="29"/>
       <c r="E179" s="29" t="s">
@@ -14745,7 +14750,7 @@
         <v>1253</v>
       </c>
       <c r="C183" s="20" t="s">
-        <v>2820</v>
+        <v>2817</v>
       </c>
       <c r="D183" s="29"/>
       <c r="E183" s="29" t="s">
@@ -14820,7 +14825,7 @@
         <v>1254</v>
       </c>
       <c r="C186" s="20" t="s">
-        <v>2821</v>
+        <v>2818</v>
       </c>
       <c r="D186" s="29"/>
       <c r="E186" s="29" t="s">
@@ -14870,7 +14875,7 @@
         <v>1255</v>
       </c>
       <c r="C188" s="31" t="s">
-        <v>2779</v>
+        <v>2776</v>
       </c>
       <c r="D188" s="29"/>
       <c r="E188" s="29" t="s">
@@ -14920,7 +14925,7 @@
         <v>1256</v>
       </c>
       <c r="C190" s="31" t="s">
-        <v>2778</v>
+        <v>2775</v>
       </c>
       <c r="D190" s="29"/>
       <c r="E190" s="29" t="s">
@@ -14970,7 +14975,7 @@
         <v>1257</v>
       </c>
       <c r="C192" s="31" t="s">
-        <v>2780</v>
+        <v>2777</v>
       </c>
       <c r="D192" s="29"/>
       <c r="E192" s="29" t="s">
@@ -15020,7 +15025,7 @@
         <v>1258</v>
       </c>
       <c r="C194" s="31" t="s">
-        <v>2781</v>
+        <v>2778</v>
       </c>
       <c r="D194" s="29"/>
       <c r="E194" s="29" t="s">
@@ -15070,7 +15075,7 @@
         <v>1259</v>
       </c>
       <c r="C196" s="20" t="s">
-        <v>2822</v>
+        <v>2819</v>
       </c>
       <c r="D196" s="29"/>
       <c r="E196" s="29" t="s">
@@ -15147,7 +15152,7 @@
         <v>1260</v>
       </c>
       <c r="C199" s="31" t="s">
-        <v>2782</v>
+        <v>2779</v>
       </c>
       <c r="D199" s="29"/>
       <c r="E199" s="29" t="s">
@@ -15222,7 +15227,7 @@
         <v>1261</v>
       </c>
       <c r="C202" s="20" t="s">
-        <v>2823</v>
+        <v>2820</v>
       </c>
       <c r="D202" s="29"/>
       <c r="E202" s="29" t="s">
@@ -15297,7 +15302,7 @@
         <v>1262</v>
       </c>
       <c r="C205" s="20" t="s">
-        <v>2824</v>
+        <v>2821</v>
       </c>
       <c r="D205" s="29"/>
       <c r="E205" s="29" t="s">
@@ -15397,7 +15402,7 @@
         <v>1263</v>
       </c>
       <c r="C209" s="20" t="s">
-        <v>2825</v>
+        <v>2822</v>
       </c>
       <c r="D209" s="29"/>
       <c r="E209" s="29" t="s">
@@ -15447,7 +15452,7 @@
         <v>1264</v>
       </c>
       <c r="C211" s="20" t="s">
-        <v>2826</v>
+        <v>2823</v>
       </c>
       <c r="D211" s="29"/>
       <c r="E211" s="29" t="s">
@@ -15524,7 +15529,7 @@
         <v>1265</v>
       </c>
       <c r="C214" s="20" t="s">
-        <v>2827</v>
+        <v>2824</v>
       </c>
       <c r="D214" s="29"/>
       <c r="E214" s="29" t="s">
@@ -15701,7 +15706,7 @@
         <v>1267</v>
       </c>
       <c r="C221" s="31" t="s">
-        <v>2783</v>
+        <v>2780</v>
       </c>
       <c r="D221" s="29"/>
       <c r="E221" s="29" t="s">
@@ -15751,7 +15756,7 @@
         <v>1268</v>
       </c>
       <c r="C223" s="31" t="s">
-        <v>2784</v>
+        <v>2781</v>
       </c>
       <c r="D223" s="29"/>
       <c r="E223" s="29" t="s">
@@ -15801,7 +15806,7 @@
         <v>1269</v>
       </c>
       <c r="C225" s="20" t="s">
-        <v>2828</v>
+        <v>2825</v>
       </c>
       <c r="D225" s="29"/>
       <c r="E225" s="29" t="s">
@@ -15878,7 +15883,7 @@
         <v>1270</v>
       </c>
       <c r="C228" s="20" t="s">
-        <v>2829</v>
+        <v>2826</v>
       </c>
       <c r="D228" s="29"/>
       <c r="E228" s="29" t="s">
@@ -15980,7 +15985,7 @@
         <v>1271</v>
       </c>
       <c r="C232" s="20" t="s">
-        <v>2830</v>
+        <v>2827</v>
       </c>
       <c r="D232" s="29"/>
       <c r="E232" s="29" t="s">
@@ -16055,7 +16060,7 @@
         <v>1272</v>
       </c>
       <c r="C235" s="31" t="s">
-        <v>2785</v>
+        <v>2782</v>
       </c>
       <c r="D235" s="29"/>
       <c r="E235" s="29" t="s">
@@ -16159,7 +16164,7 @@
         <v>1273</v>
       </c>
       <c r="C239" s="20" t="s">
-        <v>2831</v>
+        <v>2828</v>
       </c>
       <c r="D239" s="29"/>
       <c r="E239" s="29" t="s">
@@ -16209,7 +16214,7 @@
         <v>1274</v>
       </c>
       <c r="C241" s="20" t="s">
-        <v>2832</v>
+        <v>2829</v>
       </c>
       <c r="D241" s="29"/>
       <c r="E241" s="29" t="s">
@@ -16259,7 +16264,7 @@
         <v>1275</v>
       </c>
       <c r="C243" s="31" t="s">
-        <v>2786</v>
+        <v>2783</v>
       </c>
       <c r="D243" s="29"/>
       <c r="E243" s="29" t="s">
@@ -16359,7 +16364,7 @@
         <v>1276</v>
       </c>
       <c r="C247" s="20" t="s">
-        <v>2833</v>
+        <v>2830</v>
       </c>
       <c r="D247" s="29"/>
       <c r="E247" s="29" t="s">
@@ -16409,7 +16414,7 @@
         <v>1277</v>
       </c>
       <c r="C249" s="20" t="s">
-        <v>2834</v>
+        <v>2831</v>
       </c>
       <c r="D249" s="29"/>
       <c r="E249" s="29" t="s">
@@ -16484,7 +16489,7 @@
         <v>1278</v>
       </c>
       <c r="C252" s="20" t="s">
-        <v>2835</v>
+        <v>2832</v>
       </c>
       <c r="D252" s="29"/>
       <c r="E252" s="29" t="s">
@@ -16636,7 +16641,7 @@
         <v>1279</v>
       </c>
       <c r="C258" s="20" t="s">
-        <v>2836</v>
+        <v>2833</v>
       </c>
       <c r="D258" s="29"/>
       <c r="E258" s="29" t="s">
@@ -16761,7 +16766,7 @@
         <v>1280</v>
       </c>
       <c r="C263" s="20" t="s">
-        <v>2837</v>
+        <v>2834</v>
       </c>
       <c r="D263" s="29"/>
       <c r="E263" s="29" t="s">
@@ -16861,7 +16866,7 @@
         <v>1281</v>
       </c>
       <c r="C267" s="20" t="s">
-        <v>2838</v>
+        <v>2835</v>
       </c>
       <c r="D267" s="29"/>
       <c r="E267" s="29" t="s">
@@ -16986,7 +16991,7 @@
         <v>1282</v>
       </c>
       <c r="C272" s="20" t="s">
-        <v>2839</v>
+        <v>2836</v>
       </c>
       <c r="D272" s="29"/>
       <c r="E272" s="29" t="s">
@@ -17063,7 +17068,7 @@
         <v>1283</v>
       </c>
       <c r="C275" s="20" t="s">
-        <v>2840</v>
+        <v>2837</v>
       </c>
       <c r="D275" s="29"/>
       <c r="E275" s="29" t="s">
@@ -17138,7 +17143,7 @@
         <v>1284</v>
       </c>
       <c r="C278" s="20" t="s">
-        <v>2841</v>
+        <v>2838</v>
       </c>
       <c r="D278" s="29"/>
       <c r="E278" s="29" t="s">
@@ -17188,7 +17193,7 @@
         <v>1285</v>
       </c>
       <c r="C280" s="20" t="s">
-        <v>2842</v>
+        <v>2839</v>
       </c>
       <c r="D280" s="29"/>
       <c r="E280" s="29" t="s">
@@ -17238,7 +17243,7 @@
         <v>1286</v>
       </c>
       <c r="C282" s="20" t="s">
-        <v>2843</v>
+        <v>2840</v>
       </c>
       <c r="D282" s="29"/>
       <c r="E282" s="29" t="s">
@@ -17288,7 +17293,7 @@
         <v>1287</v>
       </c>
       <c r="C284" s="20" t="s">
-        <v>2844</v>
+        <v>2841</v>
       </c>
       <c r="D284" s="29"/>
       <c r="E284" s="29" t="s">
@@ -17338,7 +17343,7 @@
         <v>1288</v>
       </c>
       <c r="C286" s="20" t="s">
-        <v>2845</v>
+        <v>2842</v>
       </c>
       <c r="D286" s="29"/>
       <c r="E286" s="29" t="s">
@@ -17442,7 +17447,7 @@
         <v>1290</v>
       </c>
       <c r="C290" s="31" t="s">
-        <v>2787</v>
+        <v>2784</v>
       </c>
       <c r="D290" s="29"/>
       <c r="E290" s="29" t="s">
@@ -17519,7 +17524,7 @@
         <v>1291</v>
       </c>
       <c r="C293" s="20" t="s">
-        <v>2846</v>
+        <v>2843</v>
       </c>
       <c r="D293" s="29"/>
       <c r="E293" s="29" t="s">
@@ -17721,7 +17726,7 @@
         <v>1292</v>
       </c>
       <c r="C301" s="20" t="s">
-        <v>2847</v>
+        <v>2844</v>
       </c>
       <c r="D301" s="29"/>
       <c r="E301" s="29" t="s">
@@ -17771,7 +17776,7 @@
         <v>1293</v>
       </c>
       <c r="C303" s="20" t="s">
-        <v>2848</v>
+        <v>2845</v>
       </c>
       <c r="D303" s="29"/>
       <c r="E303" s="29" t="s">
@@ -17821,7 +17826,7 @@
         <v>1294</v>
       </c>
       <c r="C305" s="20" t="s">
-        <v>2849</v>
+        <v>2846</v>
       </c>
       <c r="D305" s="29"/>
       <c r="E305" s="29" t="s">
@@ -17871,7 +17876,7 @@
         <v>1295</v>
       </c>
       <c r="C307" s="20" t="s">
-        <v>2850</v>
+        <v>2847</v>
       </c>
       <c r="D307" s="29"/>
       <c r="E307" s="29" t="s">
@@ -17921,7 +17926,7 @@
         <v>1296</v>
       </c>
       <c r="C309" s="20" t="s">
-        <v>2851</v>
+        <v>2848</v>
       </c>
       <c r="D309" s="29"/>
       <c r="E309" s="29" t="s">
@@ -18021,7 +18026,7 @@
         <v>1297</v>
       </c>
       <c r="C313" s="20" t="s">
-        <v>2852</v>
+        <v>2849</v>
       </c>
       <c r="D313" s="29"/>
       <c r="E313" s="29" t="s">
@@ -18173,7 +18178,7 @@
         <v>1298</v>
       </c>
       <c r="C319" s="20" t="s">
-        <v>2853</v>
+        <v>2850</v>
       </c>
       <c r="D319" s="29"/>
       <c r="E319" s="29" t="s">
@@ -18248,7 +18253,7 @@
         <v>1300</v>
       </c>
       <c r="C322" s="31" t="s">
-        <v>2788</v>
+        <v>2785</v>
       </c>
       <c r="D322" s="29"/>
       <c r="E322" s="29" t="s">
@@ -18448,7 +18453,7 @@
         <v>1301</v>
       </c>
       <c r="C330" s="31" t="s">
-        <v>2789</v>
+        <v>2786</v>
       </c>
       <c r="D330" s="29"/>
       <c r="E330" s="29" t="s">
@@ -18523,7 +18528,7 @@
         <v>1302</v>
       </c>
       <c r="C333" s="31" t="s">
-        <v>2790</v>
+        <v>2787</v>
       </c>
       <c r="D333" s="29"/>
       <c r="E333" s="29" t="s">
@@ -18573,7 +18578,7 @@
         <v>1303</v>
       </c>
       <c r="C335" s="31" t="s">
-        <v>2791</v>
+        <v>2788</v>
       </c>
       <c r="D335" s="29"/>
       <c r="E335" s="29" t="s">
@@ -18873,7 +18878,7 @@
         <v>1305</v>
       </c>
       <c r="C347" s="20" t="s">
-        <v>2854</v>
+        <v>2851</v>
       </c>
       <c r="D347" s="29"/>
       <c r="E347" s="29" t="s">
@@ -18998,7 +19003,7 @@
         <v>1306</v>
       </c>
       <c r="C352" s="20" t="s">
-        <v>2855</v>
+        <v>2852</v>
       </c>
       <c r="D352" s="29"/>
       <c r="E352" s="29" t="s">
@@ -19123,7 +19128,7 @@
         <v>1307</v>
       </c>
       <c r="C357" s="20" t="s">
-        <v>2856</v>
+        <v>2853</v>
       </c>
       <c r="D357" s="29"/>
       <c r="E357" s="29" t="s">
@@ -19323,7 +19328,7 @@
         <v>1308</v>
       </c>
       <c r="C365" s="20" t="s">
-        <v>2857</v>
+        <v>2854</v>
       </c>
       <c r="D365" s="29"/>
       <c r="E365" s="29" t="s">
@@ -19525,7 +19530,7 @@
         <v>1309</v>
       </c>
       <c r="C373" s="20" t="s">
-        <v>2858</v>
+        <v>2855</v>
       </c>
       <c r="D373" s="29"/>
       <c r="E373" s="29" t="s">
@@ -19856,7 +19861,7 @@
         <v>1310</v>
       </c>
       <c r="C386" s="20" t="s">
-        <v>2859</v>
+        <v>2856</v>
       </c>
       <c r="D386" s="29"/>
       <c r="E386" s="29" t="s">
@@ -20262,7 +20267,7 @@
         <v>1311</v>
       </c>
       <c r="C402" s="20" t="s">
-        <v>2860</v>
+        <v>2857</v>
       </c>
       <c r="D402" s="29"/>
       <c r="E402" s="29" t="s">
@@ -20487,7 +20492,7 @@
         <v>1312</v>
       </c>
       <c r="C411" s="31" t="s">
-        <v>2792</v>
+        <v>2789</v>
       </c>
       <c r="D411" s="29"/>
       <c r="E411" s="29" t="s">
@@ -20681,13 +20686,13 @@
     </row>
     <row r="419" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A419" s="29" t="s">
-        <v>2794</v>
+        <v>2791</v>
       </c>
       <c r="B419" s="30" t="s">
+        <v>2790</v>
+      </c>
+      <c r="C419" s="31" t="s">
         <v>2793</v>
-      </c>
-      <c r="C419" s="31" t="s">
-        <v>2796</v>
       </c>
       <c r="D419" s="29"/>
       <c r="E419" s="29" t="s">
@@ -20706,13 +20711,13 @@
     </row>
     <row r="420" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A420" s="29" t="s">
-        <v>2795</v>
+        <v>2792</v>
       </c>
       <c r="B420" s="30" t="s">
-        <v>2793</v>
+        <v>2790</v>
       </c>
       <c r="C420" s="20" t="s">
-        <v>2861</v>
+        <v>2858</v>
       </c>
       <c r="D420" s="29"/>
       <c r="E420" s="29" t="s">
@@ -20834,7 +20839,7 @@
         <v>17</v>
       </c>
       <c r="I424" s="20" t="s">
-        <v>2701</v>
+        <v>2700</v>
       </c>
     </row>
     <row r="425" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -20945,7 +20950,7 @@
         <v>1314</v>
       </c>
       <c r="C429" s="20" t="s">
-        <v>2862</v>
+        <v>2859</v>
       </c>
       <c r="D429" s="29"/>
       <c r="E429" s="29" t="s">
@@ -21070,7 +21075,7 @@
         <v>1316</v>
       </c>
       <c r="C434" s="20" t="s">
-        <v>2863</v>
+        <v>2860</v>
       </c>
       <c r="D434" s="29"/>
       <c r="E434" s="29" t="s">
@@ -21145,7 +21150,7 @@
         <v>1317</v>
       </c>
       <c r="C437" s="20" t="s">
-        <v>2864</v>
+        <v>2861</v>
       </c>
       <c r="D437" s="29"/>
       <c r="E437" s="29" t="s">
@@ -21220,7 +21225,7 @@
         <v>1318</v>
       </c>
       <c r="C440" s="20" t="s">
-        <v>2865</v>
+        <v>2862</v>
       </c>
       <c r="D440" s="29"/>
       <c r="E440" s="29" t="s">
@@ -21324,7 +21329,7 @@
         <v>1319</v>
       </c>
       <c r="C444" s="20" t="s">
-        <v>2866</v>
+        <v>2863</v>
       </c>
       <c r="D444" s="29"/>
       <c r="E444" s="29" t="s">
@@ -21374,7 +21379,7 @@
         <v>1320</v>
       </c>
       <c r="C446" s="20" t="s">
-        <v>2867</v>
+        <v>2864</v>
       </c>
       <c r="D446" s="29"/>
       <c r="E446" s="29" t="s">
@@ -21424,7 +21429,7 @@
         <v>1321</v>
       </c>
       <c r="C448" s="20" t="s">
-        <v>2868</v>
+        <v>2865</v>
       </c>
       <c r="D448" s="29"/>
       <c r="E448" s="29" t="s">
@@ -21451,7 +21456,7 @@
         <v>1321</v>
       </c>
       <c r="C449" s="31" t="s">
-        <v>2718</v>
+        <v>2716</v>
       </c>
       <c r="D449" s="29"/>
       <c r="E449" s="29" t="s">
@@ -21620,13 +21625,13 @@
     </row>
     <row r="456" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A456" s="29" t="s">
-        <v>2719</v>
+        <v>2717</v>
       </c>
       <c r="B456" s="30" t="s">
         <v>1321</v>
       </c>
       <c r="C456" s="31" t="s">
-        <v>2720</v>
+        <v>2718</v>
       </c>
       <c r="D456" s="29"/>
       <c r="E456" s="29" t="s">
@@ -21645,13 +21650,13 @@
     </row>
     <row r="457" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A457" s="29" t="s">
-        <v>2722</v>
+        <v>2720</v>
       </c>
       <c r="B457" s="30" t="s">
         <v>1321</v>
       </c>
       <c r="C457" s="31" t="s">
-        <v>2721</v>
+        <v>2719</v>
       </c>
       <c r="D457" s="29"/>
       <c r="E457" s="29" t="s">
@@ -21701,7 +21706,7 @@
         <v>1322</v>
       </c>
       <c r="C459" s="20" t="s">
-        <v>2869</v>
+        <v>2866</v>
       </c>
       <c r="D459" s="29"/>
       <c r="E459" s="29" t="s">
@@ -21751,7 +21756,7 @@
         <v>1323</v>
       </c>
       <c r="C461" s="20" t="s">
-        <v>2870</v>
+        <v>2867</v>
       </c>
       <c r="D461" s="29"/>
       <c r="E461" s="29" t="s">
@@ -21801,7 +21806,7 @@
         <v>1324</v>
       </c>
       <c r="C463" s="20" t="s">
-        <v>2871</v>
+        <v>2868</v>
       </c>
       <c r="D463" s="29"/>
       <c r="E463" s="29" t="s">
@@ -21851,7 +21856,7 @@
         <v>1325</v>
       </c>
       <c r="C465" s="20" t="s">
-        <v>2872</v>
+        <v>2869</v>
       </c>
       <c r="D465" s="29"/>
       <c r="E465" s="29" t="s">
@@ -21901,7 +21906,7 @@
         <v>1326</v>
       </c>
       <c r="C467" s="20" t="s">
-        <v>2873</v>
+        <v>2870</v>
       </c>
       <c r="D467" s="29"/>
       <c r="E467" s="29" t="s">
@@ -21951,7 +21956,7 @@
         <v>1327</v>
       </c>
       <c r="C469" s="20" t="s">
-        <v>2874</v>
+        <v>2871</v>
       </c>
       <c r="D469" s="29"/>
       <c r="E469" s="29" t="s">
@@ -22178,7 +22183,7 @@
         <v>1328</v>
       </c>
       <c r="C478" s="20" t="s">
-        <v>2875</v>
+        <v>2872</v>
       </c>
       <c r="D478" s="29"/>
       <c r="E478" s="29" t="s">
@@ -22328,7 +22333,7 @@
         <v>1329</v>
       </c>
       <c r="C484" s="20" t="s">
-        <v>2876</v>
+        <v>2873</v>
       </c>
       <c r="D484" s="29"/>
       <c r="E484" s="29" t="s">
@@ -22378,7 +22383,7 @@
         <v>1330</v>
       </c>
       <c r="C486" s="20" t="s">
-        <v>2877</v>
+        <v>2874</v>
       </c>
       <c r="D486" s="29"/>
       <c r="E486" s="29" t="s">
@@ -22655,7 +22660,7 @@
         <v>1331</v>
       </c>
       <c r="C497" s="20" t="s">
-        <v>2878</v>
+        <v>2875</v>
       </c>
       <c r="D497" s="29"/>
       <c r="E497" s="29" t="s">
@@ -22705,7 +22710,7 @@
         <v>1332</v>
       </c>
       <c r="C499" s="20" t="s">
-        <v>2879</v>
+        <v>2876</v>
       </c>
       <c r="D499" s="29"/>
       <c r="E499" s="29" t="s">
@@ -22855,7 +22860,7 @@
         <v>1333</v>
       </c>
       <c r="C505" s="20" t="s">
-        <v>2880</v>
+        <v>2877</v>
       </c>
       <c r="D505" s="29"/>
       <c r="E505" s="29" t="s">
@@ -22930,7 +22935,7 @@
         <v>1334</v>
       </c>
       <c r="C508" s="20" t="s">
-        <v>2881</v>
+        <v>2878</v>
       </c>
       <c r="D508" s="29"/>
       <c r="E508" s="29" t="s">
@@ -23007,7 +23012,7 @@
         <v>1335</v>
       </c>
       <c r="C511" s="20" t="s">
-        <v>2882</v>
+        <v>2879</v>
       </c>
       <c r="D511" s="29"/>
       <c r="E511" s="29" t="s">
@@ -23084,7 +23089,7 @@
         <v>1336</v>
       </c>
       <c r="C514" s="20" t="s">
-        <v>2883</v>
+        <v>2880</v>
       </c>
       <c r="D514" s="29"/>
       <c r="E514" s="29" t="s">
@@ -23134,7 +23139,7 @@
         <v>1337</v>
       </c>
       <c r="C516" s="20" t="s">
-        <v>2884</v>
+        <v>2881</v>
       </c>
       <c r="D516" s="29"/>
       <c r="E516" s="29" t="s">
@@ -23178,13 +23183,13 @@
     </row>
     <row r="518" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A518" s="29" t="s">
-        <v>2728</v>
+        <v>2726</v>
       </c>
       <c r="B518" s="30" t="s">
         <v>1338</v>
       </c>
       <c r="C518" s="31" t="s">
-        <v>2723</v>
+        <v>2721</v>
       </c>
       <c r="D518" s="29"/>
       <c r="E518" s="29" t="s">
@@ -23203,13 +23208,13 @@
     </row>
     <row r="519" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A519" s="29" t="s">
-        <v>2729</v>
+        <v>2727</v>
       </c>
       <c r="B519" s="30" t="s">
         <v>1338</v>
       </c>
       <c r="C519" s="31" t="s">
-        <v>2797</v>
+        <v>2794</v>
       </c>
       <c r="D519" s="29"/>
       <c r="E519" s="29" t="s">
@@ -23228,13 +23233,13 @@
     </row>
     <row r="520" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A520" s="29" t="s">
-        <v>2730</v>
+        <v>2728</v>
       </c>
       <c r="B520" s="30" t="s">
         <v>1338</v>
       </c>
       <c r="C520" s="31" t="s">
-        <v>2724</v>
+        <v>2722</v>
       </c>
       <c r="D520" s="29"/>
       <c r="E520" s="29" t="s">
@@ -23253,13 +23258,13 @@
     </row>
     <row r="521" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A521" s="29" t="s">
-        <v>2731</v>
+        <v>2729</v>
       </c>
       <c r="B521" s="30" t="s">
         <v>1338</v>
       </c>
       <c r="C521" s="31" t="s">
-        <v>2726</v>
+        <v>2724</v>
       </c>
       <c r="D521" s="29"/>
       <c r="E521" s="29" t="s">
@@ -23278,13 +23283,13 @@
     </row>
     <row r="522" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A522" s="29" t="s">
-        <v>2732</v>
+        <v>2730</v>
       </c>
       <c r="B522" s="30" t="s">
         <v>1338</v>
       </c>
       <c r="C522" s="31" t="s">
-        <v>2725</v>
+        <v>2723</v>
       </c>
       <c r="D522" s="29"/>
       <c r="E522" s="29" t="s">
@@ -23303,13 +23308,13 @@
     </row>
     <row r="523" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A523" s="29" t="s">
-        <v>2733</v>
+        <v>2731</v>
       </c>
       <c r="B523" s="30" t="s">
         <v>1338</v>
       </c>
       <c r="C523" s="31" t="s">
-        <v>2727</v>
+        <v>2725</v>
       </c>
       <c r="D523" s="29"/>
       <c r="E523" s="29" t="s">
@@ -23328,13 +23333,13 @@
     </row>
     <row r="524" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A524" s="29" t="s">
-        <v>2750</v>
+        <v>2748</v>
       </c>
       <c r="B524" s="30" t="s">
-        <v>2734</v>
+        <v>2732</v>
       </c>
       <c r="C524" s="31" t="s">
-        <v>2735</v>
+        <v>2733</v>
       </c>
       <c r="D524" s="29"/>
       <c r="E524" s="29" t="s">
@@ -23353,13 +23358,13 @@
     </row>
     <row r="525" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A525" s="29" t="s">
-        <v>2751</v>
+        <v>2749</v>
       </c>
       <c r="B525" s="30" t="s">
-        <v>2734</v>
+        <v>2732</v>
       </c>
       <c r="C525" s="31" t="s">
-        <v>2798</v>
+        <v>2795</v>
       </c>
       <c r="D525" s="29"/>
       <c r="E525" s="29" t="s">
@@ -23378,13 +23383,13 @@
     </row>
     <row r="526" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A526" s="29" t="s">
-        <v>2752</v>
+        <v>2750</v>
       </c>
       <c r="B526" s="30" t="s">
-        <v>2734</v>
+        <v>2732</v>
       </c>
       <c r="C526" s="31" t="s">
-        <v>2746</v>
+        <v>2744</v>
       </c>
       <c r="D526" s="29"/>
       <c r="E526" s="29" t="s">
@@ -23403,13 +23408,13 @@
     </row>
     <row r="527" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A527" s="29" t="s">
-        <v>2753</v>
+        <v>2751</v>
       </c>
       <c r="B527" s="30" t="s">
-        <v>2734</v>
+        <v>2732</v>
       </c>
       <c r="C527" s="31" t="s">
-        <v>2745</v>
+        <v>2743</v>
       </c>
       <c r="D527" s="29"/>
       <c r="E527" s="29" t="s">
@@ -23428,13 +23433,13 @@
     </row>
     <row r="528" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A528" s="29" t="s">
-        <v>2754</v>
+        <v>2752</v>
       </c>
       <c r="B528" s="30" t="s">
-        <v>2734</v>
+        <v>2732</v>
       </c>
       <c r="C528" s="31" t="s">
-        <v>2744</v>
+        <v>2742</v>
       </c>
       <c r="D528" s="29"/>
       <c r="E528" s="29" t="s">
@@ -23453,13 +23458,13 @@
     </row>
     <row r="529" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A529" s="29" t="s">
-        <v>2755</v>
+        <v>2753</v>
       </c>
       <c r="B529" s="30" t="s">
-        <v>2734</v>
+        <v>2732</v>
       </c>
       <c r="C529" s="31" t="s">
-        <v>2747</v>
+        <v>2745</v>
       </c>
       <c r="D529" s="29"/>
       <c r="E529" s="29" t="s">
@@ -23478,13 +23483,13 @@
     </row>
     <row r="530" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A530" s="29" t="s">
-        <v>2756</v>
+        <v>2754</v>
       </c>
       <c r="B530" s="30" t="s">
-        <v>2734</v>
+        <v>2732</v>
       </c>
       <c r="C530" s="31" t="s">
-        <v>2748</v>
+        <v>2746</v>
       </c>
       <c r="D530" s="29"/>
       <c r="E530" s="29" t="s">
@@ -23503,13 +23508,13 @@
     </row>
     <row r="531" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A531" s="29" t="s">
-        <v>2757</v>
+        <v>2755</v>
       </c>
       <c r="B531" s="30" t="s">
-        <v>2734</v>
+        <v>2732</v>
       </c>
       <c r="C531" s="31" t="s">
-        <v>2749</v>
+        <v>2747</v>
       </c>
       <c r="D531" s="29"/>
       <c r="E531" s="29" t="s">
@@ -23528,13 +23533,13 @@
     </row>
     <row r="532" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A532" s="29" t="s">
-        <v>2758</v>
+        <v>2756</v>
       </c>
       <c r="B532" s="30" t="s">
-        <v>2736</v>
+        <v>2734</v>
       </c>
       <c r="C532" s="31" t="s">
-        <v>2737</v>
+        <v>2735</v>
       </c>
       <c r="D532" s="29"/>
       <c r="E532" s="29" t="s">
@@ -23553,13 +23558,13 @@
     </row>
     <row r="533" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A533" s="29" t="s">
-        <v>2759</v>
+        <v>2757</v>
       </c>
       <c r="B533" s="30" t="s">
-        <v>2736</v>
+        <v>2734</v>
       </c>
       <c r="C533" s="31" t="s">
-        <v>2799</v>
+        <v>2796</v>
       </c>
       <c r="D533" s="29"/>
       <c r="E533" s="29" t="s">
@@ -23578,13 +23583,13 @@
     </row>
     <row r="534" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A534" s="29" t="s">
-        <v>2760</v>
+        <v>2758</v>
       </c>
       <c r="B534" s="30" t="s">
-        <v>2736</v>
+        <v>2734</v>
       </c>
       <c r="C534" s="31" t="s">
-        <v>2740</v>
+        <v>2738</v>
       </c>
       <c r="D534" s="29"/>
       <c r="E534" s="29" t="s">
@@ -23603,13 +23608,13 @@
     </row>
     <row r="535" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A535" s="29" t="s">
-        <v>2761</v>
+        <v>2759</v>
       </c>
       <c r="B535" s="30" t="s">
-        <v>2736</v>
+        <v>2734</v>
       </c>
       <c r="C535" s="31" t="s">
-        <v>2739</v>
+        <v>2737</v>
       </c>
       <c r="D535" s="29"/>
       <c r="E535" s="29" t="s">
@@ -23628,13 +23633,13 @@
     </row>
     <row r="536" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A536" s="29" t="s">
-        <v>2762</v>
+        <v>2760</v>
       </c>
       <c r="B536" s="30" t="s">
+        <v>2734</v>
+      </c>
+      <c r="C536" s="31" t="s">
         <v>2736</v>
-      </c>
-      <c r="C536" s="31" t="s">
-        <v>2738</v>
       </c>
       <c r="D536" s="29"/>
       <c r="E536" s="29" t="s">
@@ -23653,13 +23658,13 @@
     </row>
     <row r="537" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A537" s="29" t="s">
-        <v>2763</v>
+        <v>2761</v>
       </c>
       <c r="B537" s="30" t="s">
-        <v>2736</v>
+        <v>2734</v>
       </c>
       <c r="C537" s="31" t="s">
-        <v>2741</v>
+        <v>2739</v>
       </c>
       <c r="D537" s="29"/>
       <c r="E537" s="29" t="s">
@@ -23678,13 +23683,13 @@
     </row>
     <row r="538" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A538" s="29" t="s">
-        <v>2764</v>
+        <v>2762</v>
       </c>
       <c r="B538" s="30" t="s">
-        <v>2736</v>
+        <v>2734</v>
       </c>
       <c r="C538" s="31" t="s">
-        <v>2742</v>
+        <v>2740</v>
       </c>
       <c r="D538" s="29"/>
       <c r="E538" s="29" t="s">
@@ -23703,13 +23708,13 @@
     </row>
     <row r="539" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A539" s="29" t="s">
-        <v>2765</v>
+        <v>2763</v>
       </c>
       <c r="B539" s="30" t="s">
-        <v>2736</v>
+        <v>2734</v>
       </c>
       <c r="C539" s="31" t="s">
-        <v>2743</v>
+        <v>2741</v>
       </c>
       <c r="D539" s="29"/>
       <c r="E539" s="29" t="s">
@@ -23731,7 +23736,7 @@
         <v>538</v>
       </c>
       <c r="B540" s="30" t="s">
-        <v>2766</v>
+        <v>2764</v>
       </c>
       <c r="C540" s="31" t="s">
         <v>1849</v>
@@ -23756,7 +23761,7 @@
         <v>539</v>
       </c>
       <c r="B541" s="30" t="s">
-        <v>2766</v>
+        <v>2764</v>
       </c>
       <c r="C541" s="31" t="s">
         <v>1850</v>
@@ -23783,7 +23788,7 @@
         <v>540</v>
       </c>
       <c r="B542" s="30" t="s">
-        <v>2766</v>
+        <v>2764</v>
       </c>
       <c r="C542" s="31" t="s">
         <v>1851</v>
@@ -23808,7 +23813,7 @@
         <v>541</v>
       </c>
       <c r="B543" s="30" t="s">
-        <v>2766</v>
+        <v>2764</v>
       </c>
       <c r="C543" s="31" t="s">
         <v>1852</v>
@@ -23833,7 +23838,7 @@
         <v>542</v>
       </c>
       <c r="B544" s="30" t="s">
-        <v>2766</v>
+        <v>2764</v>
       </c>
       <c r="C544" s="31" t="s">
         <v>1853</v>
@@ -23858,10 +23863,10 @@
         <v>543</v>
       </c>
       <c r="B545" s="30" t="s">
-        <v>2766</v>
+        <v>2764</v>
       </c>
       <c r="C545" s="20" t="s">
-        <v>2885</v>
+        <v>2882</v>
       </c>
       <c r="D545" s="29"/>
       <c r="E545" s="29" t="s">
@@ -23883,7 +23888,7 @@
         <v>544</v>
       </c>
       <c r="B546" s="30" t="s">
-        <v>2766</v>
+        <v>2764</v>
       </c>
       <c r="C546" s="31" t="s">
         <v>1854</v>
@@ -23908,10 +23913,10 @@
         <v>545</v>
       </c>
       <c r="B547" s="30" t="s">
-        <v>2766</v>
+        <v>2764</v>
       </c>
       <c r="C547" s="20" t="s">
-        <v>2886</v>
+        <v>2883</v>
       </c>
       <c r="D547" s="29"/>
       <c r="E547" s="29" t="s">
@@ -23933,7 +23938,7 @@
         <v>546</v>
       </c>
       <c r="B548" s="30" t="s">
-        <v>2766</v>
+        <v>2764</v>
       </c>
       <c r="C548" s="31" t="s">
         <v>1855</v>
@@ -23958,10 +23963,10 @@
         <v>547</v>
       </c>
       <c r="B549" s="30" t="s">
-        <v>2766</v>
+        <v>2764</v>
       </c>
       <c r="C549" s="20" t="s">
-        <v>2887</v>
+        <v>2884</v>
       </c>
       <c r="D549" s="29"/>
       <c r="E549" s="29" t="s">
@@ -23983,7 +23988,7 @@
         <v>548</v>
       </c>
       <c r="B550" s="30" t="s">
-        <v>2766</v>
+        <v>2764</v>
       </c>
       <c r="C550" s="31" t="s">
         <v>1856</v>
@@ -24008,7 +24013,7 @@
         <v>549</v>
       </c>
       <c r="B551" s="30" t="s">
-        <v>2766</v>
+        <v>2764</v>
       </c>
       <c r="C551" s="31" t="s">
         <v>1857</v>
@@ -24033,10 +24038,10 @@
         <v>550</v>
       </c>
       <c r="B552" s="30" t="s">
-        <v>2766</v>
+        <v>2764</v>
       </c>
       <c r="C552" s="20" t="s">
-        <v>2888</v>
+        <v>2885</v>
       </c>
       <c r="D552" s="29"/>
       <c r="E552" s="29" t="s">
@@ -24058,7 +24063,7 @@
         <v>551</v>
       </c>
       <c r="B553" s="30" t="s">
-        <v>2766</v>
+        <v>2764</v>
       </c>
       <c r="C553" s="31" t="s">
         <v>1858</v>
@@ -24083,7 +24088,7 @@
         <v>552</v>
       </c>
       <c r="B554" s="30" t="s">
-        <v>2766</v>
+        <v>2764</v>
       </c>
       <c r="C554" s="31" t="s">
         <v>1859</v>
@@ -24108,10 +24113,10 @@
         <v>553</v>
       </c>
       <c r="B555" s="30" t="s">
-        <v>2766</v>
+        <v>2764</v>
       </c>
       <c r="C555" s="20" t="s">
-        <v>2889</v>
+        <v>2886</v>
       </c>
       <c r="D555" s="29"/>
       <c r="E555" s="29" t="s">
@@ -24133,7 +24138,7 @@
         <v>554</v>
       </c>
       <c r="B556" s="30" t="s">
-        <v>2766</v>
+        <v>2764</v>
       </c>
       <c r="C556" s="31" t="s">
         <v>1860</v>
@@ -24158,10 +24163,10 @@
         <v>555</v>
       </c>
       <c r="B557" s="30" t="s">
-        <v>2766</v>
+        <v>2764</v>
       </c>
       <c r="C557" s="20" t="s">
-        <v>2890</v>
+        <v>2887</v>
       </c>
       <c r="D557" s="29"/>
       <c r="E557" s="29" t="s">
@@ -24183,7 +24188,7 @@
         <v>556</v>
       </c>
       <c r="B558" s="30" t="s">
-        <v>2766</v>
+        <v>2764</v>
       </c>
       <c r="C558" s="31" t="s">
         <v>1861</v>
@@ -24208,10 +24213,10 @@
         <v>557</v>
       </c>
       <c r="B559" s="30" t="s">
-        <v>2766</v>
+        <v>2764</v>
       </c>
       <c r="C559" s="20" t="s">
-        <v>2891</v>
+        <v>2888</v>
       </c>
       <c r="D559" s="29"/>
       <c r="E559" s="29" t="s">
@@ -24233,7 +24238,7 @@
         <v>558</v>
       </c>
       <c r="B560" s="30" t="s">
-        <v>2766</v>
+        <v>2764</v>
       </c>
       <c r="C560" s="31" t="s">
         <v>1862</v>
@@ -24258,10 +24263,10 @@
         <v>559</v>
       </c>
       <c r="B561" s="30" t="s">
-        <v>2766</v>
+        <v>2764</v>
       </c>
       <c r="C561" s="20" t="s">
-        <v>2892</v>
+        <v>2889</v>
       </c>
       <c r="D561" s="29"/>
       <c r="E561" s="29" t="s">
@@ -24283,7 +24288,7 @@
         <v>560</v>
       </c>
       <c r="B562" s="30" t="s">
-        <v>2766</v>
+        <v>2764</v>
       </c>
       <c r="C562" s="31" t="s">
         <v>1863</v>
@@ -24833,7 +24838,7 @@
         <v>17</v>
       </c>
       <c r="I583" s="20" t="s">
-        <v>2699</v>
+        <v>2698</v>
       </c>
     </row>
     <row r="584" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -26204,7 +26209,7 @@
         <v>1347</v>
       </c>
       <c r="C638" s="20" t="s">
-        <v>2705</v>
+        <v>2704</v>
       </c>
       <c r="D638" s="29"/>
       <c r="E638" s="29" t="s">
@@ -26220,7 +26225,7 @@
         <v>17</v>
       </c>
       <c r="I638" s="20" t="s">
-        <v>2706</v>
+        <v>2705</v>
       </c>
     </row>
     <row r="639" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -26325,13 +26330,13 @@
     </row>
     <row r="643" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A643" s="22" t="s">
-        <v>2704</v>
+        <v>2703</v>
       </c>
       <c r="B643" s="30" t="s">
         <v>1347</v>
       </c>
       <c r="C643" s="20" t="s">
-        <v>2707</v>
+        <v>2706</v>
       </c>
       <c r="D643" s="29"/>
       <c r="E643" s="22" t="s">
@@ -26347,7 +26352,7 @@
         <v>17</v>
       </c>
       <c r="I643" s="20" t="s">
-        <v>2710</v>
+        <v>2709</v>
       </c>
     </row>
     <row r="644" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -27591,7 +27596,7 @@
         <v>1361</v>
       </c>
       <c r="C693" s="20" t="s">
-        <v>2893</v>
+        <v>2890</v>
       </c>
       <c r="D693" s="29"/>
       <c r="E693" s="29" t="s">
@@ -28757,7 +28762,7 @@
         <v>17</v>
       </c>
       <c r="I739" s="20" t="s">
-        <v>2698</v>
+        <v>2697</v>
       </c>
     </row>
     <row r="740" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -30544,7 +30549,7 @@
         <v>17</v>
       </c>
       <c r="I810" s="20" t="s">
-        <v>2711</v>
+        <v>2710</v>
       </c>
     </row>
     <row r="811" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -33100,7 +33105,7 @@
         <v>1423</v>
       </c>
       <c r="C910" s="20" t="s">
-        <v>2894</v>
+        <v>2891</v>
       </c>
       <c r="D910" s="29"/>
       <c r="E910" s="29" t="s">
@@ -34022,7 +34027,7 @@
         <v>1433</v>
       </c>
       <c r="C946" s="20" t="s">
-        <v>2702</v>
+        <v>2701</v>
       </c>
       <c r="D946" s="29"/>
       <c r="E946" s="29" t="s">
@@ -34871,7 +34876,7 @@
         <v>17</v>
       </c>
       <c r="I979" s="31" t="s">
-        <v>2770</v>
+        <v>2767</v>
       </c>
     </row>
     <row r="980" spans="1:9" x14ac:dyDescent="0.25">
@@ -35048,7 +35053,7 @@
         <v>17</v>
       </c>
       <c r="I986" s="20" t="s">
-        <v>2717</v>
+        <v>2715</v>
       </c>
     </row>
     <row r="987" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -35531,7 +35536,7 @@
         <v>17</v>
       </c>
       <c r="I1005" s="20" t="s">
-        <v>2700</v>
+        <v>2699</v>
       </c>
     </row>
     <row r="1006" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -35839,7 +35844,7 @@
         <v>18</v>
       </c>
       <c r="I1017" s="20" t="s">
-        <v>2712</v>
+        <v>2711</v>
       </c>
     </row>
     <row r="1018" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -39277,7 +39282,7 @@
         <v>2648</v>
       </c>
       <c r="D1150" s="22" t="s">
-        <v>2713</v>
+        <v>2712</v>
       </c>
       <c r="E1150" s="29" t="s">
         <v>22</v>
@@ -39304,7 +39309,7 @@
         <v>2635</v>
       </c>
       <c r="D1151" s="22" t="s">
-        <v>2713</v>
+        <v>2712</v>
       </c>
       <c r="E1151" s="29" t="s">
         <v>22</v>
@@ -39438,7 +39443,7 @@
         <v>1236</v>
       </c>
       <c r="C1156" s="20" t="s">
-        <v>2800</v>
+        <v>2797</v>
       </c>
       <c r="D1156" s="29" t="s">
         <v>2497</v>
@@ -39499,7 +39504,7 @@
         <v>2690</v>
       </c>
       <c r="D1158" s="22" t="s">
-        <v>2708</v>
+        <v>2707</v>
       </c>
       <c r="E1158" s="29" t="s">
         <v>22</v>
@@ -39519,16 +39524,16 @@
     </row>
     <row r="1159" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A1159" s="22" t="s">
-        <v>2703</v>
+        <v>2702</v>
       </c>
       <c r="B1159" s="24" t="s">
         <v>1236</v>
       </c>
       <c r="C1159" s="20" t="s">
-        <v>2709</v>
+        <v>2708</v>
       </c>
       <c r="D1159" s="22" t="s">
-        <v>2708</v>
+        <v>2707</v>
       </c>
       <c r="E1159" s="29" t="s">
         <v>22</v>
@@ -39554,10 +39559,10 @@
         <v>1236</v>
       </c>
       <c r="C1160" s="20" t="s">
-        <v>2801</v>
+        <v>2798</v>
       </c>
       <c r="D1160" s="22" t="s">
-        <v>2697</v>
+        <v>2696</v>
       </c>
       <c r="E1160" s="29" t="s">
         <v>22</v>
@@ -39575,16 +39580,16 @@
     </row>
     <row r="1161" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A1161" s="22" t="s">
-        <v>2696</v>
+        <v>2894</v>
       </c>
       <c r="B1161" s="24" t="s">
         <v>1236</v>
       </c>
       <c r="C1161" s="20" t="s">
-        <v>2714</v>
+        <v>2895</v>
       </c>
       <c r="D1161" s="22" t="s">
-        <v>2697</v>
+        <v>2696</v>
       </c>
       <c r="E1161" s="29" t="s">
         <v>22</v>
@@ -39637,7 +39642,7 @@
         <v>1236</v>
       </c>
       <c r="C1163" s="20" t="s">
-        <v>2802</v>
+        <v>2799</v>
       </c>
       <c r="D1163" s="22" t="s">
         <v>2659</v>
@@ -39751,7 +39756,7 @@
         <v>1236</v>
       </c>
       <c r="C1167" s="31" t="s">
-        <v>2715</v>
+        <v>2713</v>
       </c>
       <c r="D1167" s="22" t="s">
         <v>2499</v>
@@ -39780,7 +39785,7 @@
         <v>1236</v>
       </c>
       <c r="C1168" s="20" t="s">
-        <v>2895</v>
+        <v>2892</v>
       </c>
       <c r="D1168" s="22" t="s">
         <v>2499</v>
@@ -39801,13 +39806,13 @@
     </row>
     <row r="1169" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A1169" s="29" t="s">
-        <v>2768</v>
+        <v>2765</v>
       </c>
       <c r="B1169" s="30" t="s">
         <v>1236</v>
       </c>
       <c r="C1169" s="31" t="s">
-        <v>2803</v>
+        <v>2800</v>
       </c>
       <c r="D1169" s="22" t="s">
         <v>2499</v>
@@ -39828,13 +39833,13 @@
     </row>
     <row r="1170" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A1170" s="29" t="s">
-        <v>2769</v>
+        <v>2766</v>
       </c>
       <c r="B1170" s="30" t="s">
         <v>1236</v>
       </c>
-      <c r="C1170" s="31" t="s">
-        <v>2767</v>
+      <c r="C1170" s="20" t="s">
+        <v>2893</v>
       </c>
       <c r="D1170" s="22" t="s">
         <v>2499</v>
@@ -40035,7 +40040,7 @@
         <v>1236</v>
       </c>
       <c r="C1177" s="31" t="s">
-        <v>2804</v>
+        <v>2801</v>
       </c>
       <c r="D1177" s="29" t="s">
         <v>2501</v>
@@ -40122,7 +40127,7 @@
         <v>1236</v>
       </c>
       <c r="C1180" s="20" t="s">
-        <v>2806</v>
+        <v>2803</v>
       </c>
       <c r="D1180" s="22" t="s">
         <v>2667</v>
@@ -40151,7 +40156,7 @@
         <v>1236</v>
       </c>
       <c r="C1181" s="20" t="s">
-        <v>2805</v>
+        <v>2802</v>
       </c>
       <c r="D1181" s="22" t="s">
         <v>2667</v>
@@ -40772,7 +40777,7 @@
         <v>1236</v>
       </c>
       <c r="C1204" s="31" t="s">
-        <v>2771</v>
+        <v>2768</v>
       </c>
       <c r="D1204" s="29"/>
       <c r="E1204" s="29" t="s">
@@ -40998,7 +41003,7 @@
         <v>1234</v>
       </c>
       <c r="C1212" s="20" t="s">
-        <v>2809</v>
+        <v>2806</v>
       </c>
       <c r="D1212" s="29"/>
       <c r="E1212" s="29" t="s">
@@ -42023,7 +42028,7 @@
         <v>1457</v>
       </c>
       <c r="C1253" s="31" t="s">
-        <v>2772</v>
+        <v>2769</v>
       </c>
       <c r="D1253" s="29"/>
       <c r="E1253" s="29" t="s">

</xml_diff>

<commit_message>
MS-OXCMSG: Update RS and Test Suites.
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCMSG/MS-OXCMSG_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCMSG/MS-OXCMSG_RequirementSpecification.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47EA9322-68BC-40B5-8D8F-2A69ABA24C98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7789B9AE-519A-46E5-BA29-02A110EA5EBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8992" uniqueCount="2896">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8992" uniqueCount="2897">
   <si>
     <t>Req ID</t>
   </si>
@@ -9036,6 +9036,10 @@
   </si>
   <si>
     <t>[In Appendix A: Product Behavior] [PartialCompletion] A nonzero value indicates the server was unable to modify one or more of the Message objects represented in the MessageIds field. (Exchange 2007 follows this behavior.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test Case</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -9309,21 +9313,6 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -9347,6 +9336,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -10295,9 +10299,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L1258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1158" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1162" sqref="C1162"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10351,127 +10353,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -10484,12 +10486,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -10502,12 +10504,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -10520,12 +10522,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -10538,60 +10540,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="41"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="45"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -23626,8 +23628,8 @@
       <c r="G535" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="H535" s="29" t="s">
-        <v>18</v>
+      <c r="H535" s="22" t="s">
+        <v>2896</v>
       </c>
       <c r="I535" s="31"/>
     </row>
@@ -42130,6 +42132,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -42137,11 +42144,6 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A638:H638 A20:I31 A32:H32 A639:I1256 A33:I637">
@@ -42252,18 +42254,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -42316,6 +42318,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -42325,14 +42335,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Update RS and Code for release 20240220
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCMSG/MS-OXCMSG_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCMSG/MS-OXCMSG_RequirementSpecification.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26CEFE25-C1B8-4C95-80CF-D2FF1F047F47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8C8387-20CA-4FF4-8DF3-AD893690977F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$19:$G$1256</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$D$3:$I$11</definedName>
     <definedName name="ExtensionList">Requirements!#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Requirements!$A:$A,Requirements!$19:$19</definedName>
     <definedName name="ScopeList">Requirements!#REF!</definedName>
@@ -8658,12 +8658,6 @@
     <t>[In Appendix A: Product Behavior] Implementation does return Success for RopSaveChangesMessage ROP requests ([MS-OXCROPS] section 2.2.6.3) when a previous request has already been committed against the Message object, even though the changes to the object are not actually committed to the server message store. (Exchange 2010, Exchange 2013 and Exchange 2016 follow this behavior.)</t>
   </si>
   <si>
-    <t>[In Appendix A: Product Behavior] [ecError (0x80004005)] The message has been opened or previously saved as read only; changes cannot be saved. (&lt;27&gt; Section 3.2.5.3: Exchange 2007 and Exchange 2019 return Success. )</t>
-  </si>
-  <si>
-    <t>[In Appendix A: Product Behavior] [ecError (0x80004005)] The message has been opened or previously saved as read only; changes cannot be saved. (&lt;27&gt; Section 3.2.5.3: Exchange 2010, Exchange 2013 and Exchange 2016 follow this behavior.)</t>
-  </si>
-  <si>
     <t>[In PidTagHasAttachments Property] The PidTagHasAttachments property ([MS-OXPROPS] section 2.716) indicates whether the Message object contains at least one attachment.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -9027,9 +9021,6 @@
     <t>MS-OXCMSG</t>
   </si>
   <si>
-    <t>25.2</t>
-  </si>
-  <si>
     <t>[In PidTagSubjectPrefix Property] The PidTagSubjectPrefix property ([MS-OXPROPS] section 2.1034) contains the prefix for the subject of the message.</t>
   </si>
   <si>
@@ -9037,6 +9028,15 @@
   </si>
   <si>
     <t>[In PidTagArchiveTag Property] The PidTagArchiveTag property ([MS-OXPROPS] section 2.581) specifies the GUID of an archive tag. The PidTagArchiveTag property can be present on both Message objects and folders and can be set by both client and server.</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] [ecError (0x80004005)] The message has been opened or previously saved as read only; changes cannot be saved. (&lt;27&gt; Section 3.2.5.3: Exchange 2007, Exchange 2016 and Exchange 2019 return Success. )</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] [ecError (0x80004005)] The message has been opened or previously saved as read only; changes cannot be saved. (&lt;27&gt; Section 3.2.5.3: Exchange 2010, Exchange 2013 follow this behavior.)</t>
+  </si>
+  <si>
+    <t>25.3</t>
   </si>
 </sst>
 </file>
@@ -9303,6 +9303,21 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -9327,46 +9342,11 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="39">
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
+  <dxfs count="33">
     <dxf>
       <font>
         <strike/>
@@ -9420,16 +9400,6 @@
           <bgColor theme="5" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -9918,34 +9888,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I1256" tableType="xml" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37" connectionId="1">
-  <autoFilter ref="A19:I1256" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I1256" tableType="xml" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31" connectionId="1">
+  <autoFilter ref="A19:I1256" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="36">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="30">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="35">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="29">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="ns1:Description" name="Description" dataDxfId="34">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="ns1:Description" name="Description" dataDxfId="28">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="ns1:Derived" name="Derived" dataDxfId="33">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="ns1:Derived" name="Derived" dataDxfId="27">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="32">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="26">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="ns1:Scope" name="Scope" dataDxfId="31">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="ns1:Scope" name="Scope" dataDxfId="25">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="30">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="24">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="ns1:Verification" name="Verification" dataDxfId="29">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="ns1:Verification" name="Verification" dataDxfId="23">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="28">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="22">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -9954,12 +9924,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26" tableBorderDxfId="24" totalsRowBorderDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18" totalsRowBorderDxfId="17">
   <autoFilter ref="A12:C15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Scope" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Scope" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -10255,8 +10225,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J1258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -10276,7 +10246,7 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>2892</v>
+        <v>2890</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>27</v>
@@ -10299,138 +10269,138 @@
         <v>25</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>2893</v>
+        <v>2896</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>26</v>
       </c>
       <c r="F3" s="9">
-        <v>45243</v>
+        <v>45342</v>
       </c>
       <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
       <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
       <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
       <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
       <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
       <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
       <c r="J9" s="4"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
       <c r="J10" s="4"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
       <c r="J11" s="4"/>
     </row>
     <row r="12" spans="1:10">
@@ -10443,12 +10413,12 @@
       <c r="C12" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="35"/>
       <c r="J12" s="4"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -10461,12 +10431,12 @@
       <c r="C13" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
       <c r="J13" s="4"/>
     </row>
     <row r="14" spans="1:10">
@@ -10479,12 +10449,12 @@
       <c r="C14" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
       <c r="J14" s="4"/>
     </row>
     <row r="15" spans="1:10">
@@ -10497,60 +10467,60 @@
       <c r="C15" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
       <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
       <c r="J16" s="4"/>
     </row>
     <row r="17" spans="1:10" ht="64.5" customHeight="1">
       <c r="A17" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="35" t="s">
+      <c r="B17" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="36"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
       <c r="J17" s="4"/>
     </row>
     <row r="18" spans="1:10" ht="30" customHeight="1">
       <c r="A18" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="29" t="s">
+      <c r="B18" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
       <c r="J18" s="4"/>
     </row>
     <row r="19" spans="1:10" ht="29">
@@ -11264,7 +11234,7 @@
         <v>1234</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>2802</v>
+        <v>2800</v>
       </c>
       <c r="D46" s="25"/>
       <c r="E46" s="25" t="s">
@@ -11339,7 +11309,7 @@
         <v>1234</v>
       </c>
       <c r="C49" s="17" t="s">
-        <v>2804</v>
+        <v>2802</v>
       </c>
       <c r="D49" s="25"/>
       <c r="E49" s="25" t="s">
@@ -11389,7 +11359,7 @@
         <v>1235</v>
       </c>
       <c r="C51" s="17" t="s">
-        <v>2805</v>
+        <v>2803</v>
       </c>
       <c r="D51" s="25"/>
       <c r="E51" s="25" t="s">
@@ -11666,7 +11636,7 @@
         <v>1237</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>2806</v>
+        <v>2804</v>
       </c>
       <c r="D62" s="25"/>
       <c r="E62" s="25" t="s">
@@ -11816,7 +11786,7 @@
         <v>1239</v>
       </c>
       <c r="C68" s="17" t="s">
-        <v>2807</v>
+        <v>2805</v>
       </c>
       <c r="D68" s="25"/>
       <c r="E68" s="25" t="s">
@@ -12849,7 +12819,7 @@
         <v>1242</v>
       </c>
       <c r="C109" s="17" t="s">
-        <v>2894</v>
+        <v>2891</v>
       </c>
       <c r="D109" s="25"/>
       <c r="E109" s="25" t="s">
@@ -12974,7 +12944,7 @@
         <v>1243</v>
       </c>
       <c r="C114" s="17" t="s">
-        <v>2808</v>
+        <v>2806</v>
       </c>
       <c r="D114" s="25"/>
       <c r="E114" s="25" t="s">
@@ -13099,7 +13069,7 @@
         <v>1244</v>
       </c>
       <c r="C119" s="17" t="s">
-        <v>2809</v>
+        <v>2807</v>
       </c>
       <c r="D119" s="25"/>
       <c r="E119" s="25" t="s">
@@ -13251,7 +13221,7 @@
         <v>1245</v>
       </c>
       <c r="C125" s="17" t="s">
-        <v>2810</v>
+        <v>2808</v>
       </c>
       <c r="D125" s="25"/>
       <c r="E125" s="25" t="s">
@@ -13403,7 +13373,7 @@
         <v>1246</v>
       </c>
       <c r="C131" s="17" t="s">
-        <v>2811</v>
+        <v>2809</v>
       </c>
       <c r="D131" s="25"/>
       <c r="E131" s="25" t="s">
@@ -14432,7 +14402,7 @@
         <v>1250</v>
       </c>
       <c r="C172" s="17" t="s">
-        <v>2812</v>
+        <v>2810</v>
       </c>
       <c r="D172" s="25"/>
       <c r="E172" s="25" t="s">
@@ -14707,7 +14677,7 @@
         <v>1253</v>
       </c>
       <c r="C183" s="17" t="s">
-        <v>2813</v>
+        <v>2811</v>
       </c>
       <c r="D183" s="25"/>
       <c r="E183" s="25" t="s">
@@ -14782,7 +14752,7 @@
         <v>1254</v>
       </c>
       <c r="C186" s="17" t="s">
-        <v>2814</v>
+        <v>2812</v>
       </c>
       <c r="D186" s="25"/>
       <c r="E186" s="25" t="s">
@@ -15032,7 +15002,7 @@
         <v>1259</v>
       </c>
       <c r="C196" s="17" t="s">
-        <v>2815</v>
+        <v>2813</v>
       </c>
       <c r="D196" s="25"/>
       <c r="E196" s="25" t="s">
@@ -15184,7 +15154,7 @@
         <v>1261</v>
       </c>
       <c r="C202" s="17" t="s">
-        <v>2816</v>
+        <v>2814</v>
       </c>
       <c r="D202" s="25"/>
       <c r="E202" s="25" t="s">
@@ -15259,7 +15229,7 @@
         <v>1262</v>
       </c>
       <c r="C205" s="17" t="s">
-        <v>2817</v>
+        <v>2815</v>
       </c>
       <c r="D205" s="25"/>
       <c r="E205" s="25" t="s">
@@ -15359,7 +15329,7 @@
         <v>1263</v>
       </c>
       <c r="C209" s="17" t="s">
-        <v>2818</v>
+        <v>2816</v>
       </c>
       <c r="D209" s="25"/>
       <c r="E209" s="25" t="s">
@@ -15409,7 +15379,7 @@
         <v>1264</v>
       </c>
       <c r="C211" s="17" t="s">
-        <v>2819</v>
+        <v>2817</v>
       </c>
       <c r="D211" s="25"/>
       <c r="E211" s="25" t="s">
@@ -15486,7 +15456,7 @@
         <v>1265</v>
       </c>
       <c r="C214" s="17" t="s">
-        <v>2820</v>
+        <v>2818</v>
       </c>
       <c r="D214" s="25"/>
       <c r="E214" s="25" t="s">
@@ -15763,7 +15733,7 @@
         <v>1269</v>
       </c>
       <c r="C225" s="17" t="s">
-        <v>2821</v>
+        <v>2819</v>
       </c>
       <c r="D225" s="25"/>
       <c r="E225" s="25" t="s">
@@ -15840,7 +15810,7 @@
         <v>1270</v>
       </c>
       <c r="C228" s="17" t="s">
-        <v>2822</v>
+        <v>2820</v>
       </c>
       <c r="D228" s="25"/>
       <c r="E228" s="25" t="s">
@@ -15942,7 +15912,7 @@
         <v>1271</v>
       </c>
       <c r="C232" s="17" t="s">
-        <v>2823</v>
+        <v>2821</v>
       </c>
       <c r="D232" s="25"/>
       <c r="E232" s="25" t="s">
@@ -16121,7 +16091,7 @@
         <v>1273</v>
       </c>
       <c r="C239" s="17" t="s">
-        <v>2824</v>
+        <v>2822</v>
       </c>
       <c r="D239" s="25"/>
       <c r="E239" s="25" t="s">
@@ -16171,7 +16141,7 @@
         <v>1274</v>
       </c>
       <c r="C241" s="17" t="s">
-        <v>2825</v>
+        <v>2823</v>
       </c>
       <c r="D241" s="25"/>
       <c r="E241" s="25" t="s">
@@ -16321,7 +16291,7 @@
         <v>1276</v>
       </c>
       <c r="C247" s="17" t="s">
-        <v>2826</v>
+        <v>2824</v>
       </c>
       <c r="D247" s="25"/>
       <c r="E247" s="25" t="s">
@@ -16371,7 +16341,7 @@
         <v>1277</v>
       </c>
       <c r="C249" s="17" t="s">
-        <v>2827</v>
+        <v>2825</v>
       </c>
       <c r="D249" s="25"/>
       <c r="E249" s="25" t="s">
@@ -16446,7 +16416,7 @@
         <v>1278</v>
       </c>
       <c r="C252" s="17" t="s">
-        <v>2828</v>
+        <v>2826</v>
       </c>
       <c r="D252" s="25"/>
       <c r="E252" s="25" t="s">
@@ -16598,7 +16568,7 @@
         <v>1279</v>
       </c>
       <c r="C258" s="17" t="s">
-        <v>2829</v>
+        <v>2827</v>
       </c>
       <c r="D258" s="25"/>
       <c r="E258" s="25" t="s">
@@ -16723,7 +16693,7 @@
         <v>1280</v>
       </c>
       <c r="C263" s="17" t="s">
-        <v>2830</v>
+        <v>2828</v>
       </c>
       <c r="D263" s="25"/>
       <c r="E263" s="25" t="s">
@@ -16823,7 +16793,7 @@
         <v>1281</v>
       </c>
       <c r="C267" s="17" t="s">
-        <v>2831</v>
+        <v>2829</v>
       </c>
       <c r="D267" s="25"/>
       <c r="E267" s="25" t="s">
@@ -16948,7 +16918,7 @@
         <v>1282</v>
       </c>
       <c r="C272" s="17" t="s">
-        <v>2832</v>
+        <v>2830</v>
       </c>
       <c r="D272" s="25"/>
       <c r="E272" s="25" t="s">
@@ -17025,7 +16995,7 @@
         <v>1283</v>
       </c>
       <c r="C275" s="17" t="s">
-        <v>2833</v>
+        <v>2831</v>
       </c>
       <c r="D275" s="25"/>
       <c r="E275" s="25" t="s">
@@ -17100,7 +17070,7 @@
         <v>1284</v>
       </c>
       <c r="C278" s="17" t="s">
-        <v>2834</v>
+        <v>2832</v>
       </c>
       <c r="D278" s="25"/>
       <c r="E278" s="25" t="s">
@@ -17150,7 +17120,7 @@
         <v>1285</v>
       </c>
       <c r="C280" s="17" t="s">
-        <v>2835</v>
+        <v>2833</v>
       </c>
       <c r="D280" s="25"/>
       <c r="E280" s="25" t="s">
@@ -17200,7 +17170,7 @@
         <v>1286</v>
       </c>
       <c r="C282" s="17" t="s">
-        <v>2836</v>
+        <v>2834</v>
       </c>
       <c r="D282" s="25"/>
       <c r="E282" s="25" t="s">
@@ -17250,7 +17220,7 @@
         <v>1287</v>
       </c>
       <c r="C284" s="17" t="s">
-        <v>2837</v>
+        <v>2835</v>
       </c>
       <c r="D284" s="25"/>
       <c r="E284" s="25" t="s">
@@ -17300,7 +17270,7 @@
         <v>1288</v>
       </c>
       <c r="C286" s="17" t="s">
-        <v>2838</v>
+        <v>2836</v>
       </c>
       <c r="D286" s="25"/>
       <c r="E286" s="25" t="s">
@@ -17481,7 +17451,7 @@
         <v>1291</v>
       </c>
       <c r="C293" s="17" t="s">
-        <v>2839</v>
+        <v>2837</v>
       </c>
       <c r="D293" s="25"/>
       <c r="E293" s="25" t="s">
@@ -17683,7 +17653,7 @@
         <v>1292</v>
       </c>
       <c r="C301" s="17" t="s">
-        <v>2840</v>
+        <v>2838</v>
       </c>
       <c r="D301" s="25"/>
       <c r="E301" s="25" t="s">
@@ -17733,7 +17703,7 @@
         <v>1293</v>
       </c>
       <c r="C303" s="17" t="s">
-        <v>2841</v>
+        <v>2839</v>
       </c>
       <c r="D303" s="25"/>
       <c r="E303" s="25" t="s">
@@ -17783,7 +17753,7 @@
         <v>1294</v>
       </c>
       <c r="C305" s="17" t="s">
-        <v>2842</v>
+        <v>2840</v>
       </c>
       <c r="D305" s="25"/>
       <c r="E305" s="25" t="s">
@@ -17833,7 +17803,7 @@
         <v>1295</v>
       </c>
       <c r="C307" s="17" t="s">
-        <v>2843</v>
+        <v>2841</v>
       </c>
       <c r="D307" s="25"/>
       <c r="E307" s="25" t="s">
@@ -17883,7 +17853,7 @@
         <v>1296</v>
       </c>
       <c r="C309" s="17" t="s">
-        <v>2844</v>
+        <v>2842</v>
       </c>
       <c r="D309" s="25"/>
       <c r="E309" s="25" t="s">
@@ -17983,7 +17953,7 @@
         <v>1297</v>
       </c>
       <c r="C313" s="17" t="s">
-        <v>2845</v>
+        <v>2843</v>
       </c>
       <c r="D313" s="25"/>
       <c r="E313" s="25" t="s">
@@ -18135,7 +18105,7 @@
         <v>1298</v>
       </c>
       <c r="C319" s="17" t="s">
-        <v>2846</v>
+        <v>2844</v>
       </c>
       <c r="D319" s="25"/>
       <c r="E319" s="25" t="s">
@@ -18635,7 +18605,7 @@
         <v>1303</v>
       </c>
       <c r="C339" s="17" t="s">
-        <v>2895</v>
+        <v>2892</v>
       </c>
       <c r="D339" s="25"/>
       <c r="E339" s="25" t="s">
@@ -18835,7 +18805,7 @@
         <v>1305</v>
       </c>
       <c r="C347" s="17" t="s">
-        <v>2896</v>
+        <v>2893</v>
       </c>
       <c r="D347" s="25"/>
       <c r="E347" s="25" t="s">
@@ -18960,7 +18930,7 @@
         <v>1306</v>
       </c>
       <c r="C352" s="17" t="s">
-        <v>2847</v>
+        <v>2845</v>
       </c>
       <c r="D352" s="25"/>
       <c r="E352" s="25" t="s">
@@ -19085,7 +19055,7 @@
         <v>1307</v>
       </c>
       <c r="C357" s="17" t="s">
-        <v>2848</v>
+        <v>2846</v>
       </c>
       <c r="D357" s="25"/>
       <c r="E357" s="25" t="s">
@@ -19285,7 +19255,7 @@
         <v>1308</v>
       </c>
       <c r="C365" s="17" t="s">
-        <v>2849</v>
+        <v>2847</v>
       </c>
       <c r="D365" s="25"/>
       <c r="E365" s="25" t="s">
@@ -19487,7 +19457,7 @@
         <v>1309</v>
       </c>
       <c r="C373" s="17" t="s">
-        <v>2850</v>
+        <v>2848</v>
       </c>
       <c r="D373" s="25"/>
       <c r="E373" s="25" t="s">
@@ -19818,7 +19788,7 @@
         <v>1310</v>
       </c>
       <c r="C386" s="17" t="s">
-        <v>2851</v>
+        <v>2849</v>
       </c>
       <c r="D386" s="25"/>
       <c r="E386" s="25" t="s">
@@ -20224,7 +20194,7 @@
         <v>1311</v>
       </c>
       <c r="C402" s="17" t="s">
-        <v>2852</v>
+        <v>2850</v>
       </c>
       <c r="D402" s="25"/>
       <c r="E402" s="25" t="s">
@@ -20674,7 +20644,7 @@
         <v>2788</v>
       </c>
       <c r="C420" s="17" t="s">
-        <v>2853</v>
+        <v>2851</v>
       </c>
       <c r="D420" s="25"/>
       <c r="E420" s="25" t="s">
@@ -20907,7 +20877,7 @@
         <v>1314</v>
       </c>
       <c r="C429" s="17" t="s">
-        <v>2854</v>
+        <v>2852</v>
       </c>
       <c r="D429" s="25"/>
       <c r="E429" s="25" t="s">
@@ -21032,7 +21002,7 @@
         <v>1316</v>
       </c>
       <c r="C434" s="17" t="s">
-        <v>2855</v>
+        <v>2853</v>
       </c>
       <c r="D434" s="25"/>
       <c r="E434" s="25" t="s">
@@ -21107,7 +21077,7 @@
         <v>1317</v>
       </c>
       <c r="C437" s="17" t="s">
-        <v>2856</v>
+        <v>2854</v>
       </c>
       <c r="D437" s="25"/>
       <c r="E437" s="25" t="s">
@@ -21182,7 +21152,7 @@
         <v>1318</v>
       </c>
       <c r="C440" s="17" t="s">
-        <v>2857</v>
+        <v>2855</v>
       </c>
       <c r="D440" s="25"/>
       <c r="E440" s="25" t="s">
@@ -21286,7 +21256,7 @@
         <v>1319</v>
       </c>
       <c r="C444" s="17" t="s">
-        <v>2858</v>
+        <v>2856</v>
       </c>
       <c r="D444" s="25"/>
       <c r="E444" s="25" t="s">
@@ -21336,7 +21306,7 @@
         <v>1320</v>
       </c>
       <c r="C446" s="17" t="s">
-        <v>2859</v>
+        <v>2857</v>
       </c>
       <c r="D446" s="25"/>
       <c r="E446" s="25" t="s">
@@ -21386,7 +21356,7 @@
         <v>1321</v>
       </c>
       <c r="C448" s="17" t="s">
-        <v>2860</v>
+        <v>2858</v>
       </c>
       <c r="D448" s="25"/>
       <c r="E448" s="25" t="s">
@@ -21663,7 +21633,7 @@
         <v>1322</v>
       </c>
       <c r="C459" s="17" t="s">
-        <v>2861</v>
+        <v>2859</v>
       </c>
       <c r="D459" s="25"/>
       <c r="E459" s="25" t="s">
@@ -21713,7 +21683,7 @@
         <v>1323</v>
       </c>
       <c r="C461" s="17" t="s">
-        <v>2862</v>
+        <v>2860</v>
       </c>
       <c r="D461" s="25"/>
       <c r="E461" s="25" t="s">
@@ -21763,7 +21733,7 @@
         <v>1324</v>
       </c>
       <c r="C463" s="17" t="s">
-        <v>2863</v>
+        <v>2861</v>
       </c>
       <c r="D463" s="25"/>
       <c r="E463" s="25" t="s">
@@ -21813,7 +21783,7 @@
         <v>1325</v>
       </c>
       <c r="C465" s="17" t="s">
-        <v>2864</v>
+        <v>2862</v>
       </c>
       <c r="D465" s="25"/>
       <c r="E465" s="25" t="s">
@@ -21863,7 +21833,7 @@
         <v>1326</v>
       </c>
       <c r="C467" s="17" t="s">
-        <v>2865</v>
+        <v>2863</v>
       </c>
       <c r="D467" s="25"/>
       <c r="E467" s="25" t="s">
@@ -21913,7 +21883,7 @@
         <v>1327</v>
       </c>
       <c r="C469" s="17" t="s">
-        <v>2866</v>
+        <v>2864</v>
       </c>
       <c r="D469" s="25"/>
       <c r="E469" s="25" t="s">
@@ -22140,7 +22110,7 @@
         <v>1328</v>
       </c>
       <c r="C478" s="17" t="s">
-        <v>2867</v>
+        <v>2865</v>
       </c>
       <c r="D478" s="25"/>
       <c r="E478" s="25" t="s">
@@ -22290,7 +22260,7 @@
         <v>1329</v>
       </c>
       <c r="C484" s="17" t="s">
-        <v>2868</v>
+        <v>2866</v>
       </c>
       <c r="D484" s="25"/>
       <c r="E484" s="25" t="s">
@@ -22340,7 +22310,7 @@
         <v>1330</v>
       </c>
       <c r="C486" s="17" t="s">
-        <v>2869</v>
+        <v>2867</v>
       </c>
       <c r="D486" s="25"/>
       <c r="E486" s="25" t="s">
@@ -22617,7 +22587,7 @@
         <v>1331</v>
       </c>
       <c r="C497" s="17" t="s">
-        <v>2870</v>
+        <v>2868</v>
       </c>
       <c r="D497" s="25"/>
       <c r="E497" s="25" t="s">
@@ -22667,7 +22637,7 @@
         <v>1332</v>
       </c>
       <c r="C499" s="17" t="s">
-        <v>2871</v>
+        <v>2869</v>
       </c>
       <c r="D499" s="25"/>
       <c r="E499" s="25" t="s">
@@ -22817,7 +22787,7 @@
         <v>1333</v>
       </c>
       <c r="C505" s="17" t="s">
-        <v>2872</v>
+        <v>2870</v>
       </c>
       <c r="D505" s="25"/>
       <c r="E505" s="25" t="s">
@@ -22892,7 +22862,7 @@
         <v>1334</v>
       </c>
       <c r="C508" s="17" t="s">
-        <v>2873</v>
+        <v>2871</v>
       </c>
       <c r="D508" s="25"/>
       <c r="E508" s="25" t="s">
@@ -22969,7 +22939,7 @@
         <v>1335</v>
       </c>
       <c r="C511" s="17" t="s">
-        <v>2874</v>
+        <v>2872</v>
       </c>
       <c r="D511" s="25"/>
       <c r="E511" s="25" t="s">
@@ -23046,7 +23016,7 @@
         <v>1336</v>
       </c>
       <c r="C514" s="17" t="s">
-        <v>2875</v>
+        <v>2873</v>
       </c>
       <c r="D514" s="25"/>
       <c r="E514" s="25" t="s">
@@ -23096,7 +23066,7 @@
         <v>1337</v>
       </c>
       <c r="C516" s="17" t="s">
-        <v>2876</v>
+        <v>2874</v>
       </c>
       <c r="D516" s="25"/>
       <c r="E516" s="25" t="s">
@@ -23584,7 +23554,7 @@
         <v>15</v>
       </c>
       <c r="H535" s="18" t="s">
-        <v>2891</v>
+        <v>2889</v>
       </c>
       <c r="I535" s="27"/>
     </row>
@@ -23823,7 +23793,7 @@
         <v>2762</v>
       </c>
       <c r="C545" s="17" t="s">
-        <v>2877</v>
+        <v>2875</v>
       </c>
       <c r="D545" s="25"/>
       <c r="E545" s="25" t="s">
@@ -23873,7 +23843,7 @@
         <v>2762</v>
       </c>
       <c r="C547" s="17" t="s">
-        <v>2878</v>
+        <v>2876</v>
       </c>
       <c r="D547" s="25"/>
       <c r="E547" s="25" t="s">
@@ -23923,7 +23893,7 @@
         <v>2762</v>
       </c>
       <c r="C549" s="17" t="s">
-        <v>2879</v>
+        <v>2877</v>
       </c>
       <c r="D549" s="25"/>
       <c r="E549" s="25" t="s">
@@ -23998,7 +23968,7 @@
         <v>2762</v>
       </c>
       <c r="C552" s="17" t="s">
-        <v>2880</v>
+        <v>2878</v>
       </c>
       <c r="D552" s="25"/>
       <c r="E552" s="25" t="s">
@@ -24073,7 +24043,7 @@
         <v>2762</v>
       </c>
       <c r="C555" s="17" t="s">
-        <v>2881</v>
+        <v>2879</v>
       </c>
       <c r="D555" s="25"/>
       <c r="E555" s="25" t="s">
@@ -24123,7 +24093,7 @@
         <v>2762</v>
       </c>
       <c r="C557" s="17" t="s">
-        <v>2882</v>
+        <v>2880</v>
       </c>
       <c r="D557" s="25"/>
       <c r="E557" s="25" t="s">
@@ -24173,7 +24143,7 @@
         <v>2762</v>
       </c>
       <c r="C559" s="17" t="s">
-        <v>2883</v>
+        <v>2881</v>
       </c>
       <c r="D559" s="25"/>
       <c r="E559" s="25" t="s">
@@ -24223,7 +24193,7 @@
         <v>2762</v>
       </c>
       <c r="C561" s="17" t="s">
-        <v>2884</v>
+        <v>2882</v>
       </c>
       <c r="D561" s="25"/>
       <c r="E561" s="25" t="s">
@@ -27553,7 +27523,7 @@
         <v>1361</v>
       </c>
       <c r="C693" s="17" t="s">
-        <v>2885</v>
+        <v>2883</v>
       </c>
       <c r="D693" s="25"/>
       <c r="E693" s="25" t="s">
@@ -33062,7 +33032,7 @@
         <v>1423</v>
       </c>
       <c r="C910" s="17" t="s">
-        <v>2886</v>
+        <v>2884</v>
       </c>
       <c r="D910" s="25"/>
       <c r="E910" s="25" t="s">
@@ -39537,13 +39507,13 @@
     </row>
     <row r="1161" spans="1:9" ht="43.5">
       <c r="A1161" s="18" t="s">
-        <v>2889</v>
+        <v>2887</v>
       </c>
       <c r="B1161" s="20" t="s">
         <v>1236</v>
       </c>
       <c r="C1161" s="17" t="s">
-        <v>2890</v>
+        <v>2888</v>
       </c>
       <c r="D1161" s="18" t="s">
         <v>2694</v>
@@ -39742,7 +39712,7 @@
         <v>1236</v>
       </c>
       <c r="C1168" s="17" t="s">
-        <v>2887</v>
+        <v>2885</v>
       </c>
       <c r="D1168" s="18" t="s">
         <v>2498</v>
@@ -39796,7 +39766,7 @@
         <v>1236</v>
       </c>
       <c r="C1170" s="17" t="s">
-        <v>2888</v>
+        <v>2886</v>
       </c>
       <c r="D1170" s="18" t="s">
         <v>2498</v>
@@ -40084,7 +40054,7 @@
         <v>1236</v>
       </c>
       <c r="C1180" s="17" t="s">
-        <v>2801</v>
+        <v>2895</v>
       </c>
       <c r="D1180" s="18" t="s">
         <v>2665</v>
@@ -40113,7 +40083,7 @@
         <v>1236</v>
       </c>
       <c r="C1181" s="17" t="s">
-        <v>2800</v>
+        <v>2894</v>
       </c>
       <c r="D1181" s="18" t="s">
         <v>2665</v>
@@ -40960,7 +40930,7 @@
         <v>1234</v>
       </c>
       <c r="C1212" s="17" t="s">
-        <v>2803</v>
+        <v>2801</v>
       </c>
       <c r="D1212" s="25"/>
       <c r="E1212" s="25" t="s">
@@ -42084,12 +42054,8 @@
       <c r="B1258" s="8"/>
     </row>
   </sheetData>
+  <autoFilter ref="D3:I11" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -42097,80 +42063,61 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A638:H638 A20:I31 A32:H32 A639:I1256 A33:I637">
-    <cfRule type="expression" dxfId="19" priority="65">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+  <conditionalFormatting sqref="A20:I31 A32:H32 A33:I637 A638:H638 A639:I1256">
+    <cfRule type="expression" dxfId="13" priority="19">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="66">
+    <cfRule type="expression" dxfId="12" priority="20">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="73">
+    <cfRule type="expression" dxfId="11" priority="21">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A638:H638 A20:I31 A32:H32 A639:I1256 A33:I637">
-    <cfRule type="expression" dxfId="16" priority="19">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="15" priority="20">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="21">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    <cfRule type="expression" dxfId="10" priority="65">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:F1256">
-    <cfRule type="expression" dxfId="13" priority="25">
+    <cfRule type="expression" dxfId="9" priority="25">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="26">
+    <cfRule type="expression" dxfId="8" priority="26">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I638">
-    <cfRule type="expression" dxfId="11" priority="10">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+  <conditionalFormatting sqref="I32">
+    <cfRule type="expression" dxfId="7" priority="1">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="11">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="12">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="4">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I638">
-    <cfRule type="expression" dxfId="8" priority="7">
+    <cfRule type="expression" dxfId="3" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="2" priority="8">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="9">
+    <cfRule type="expression" dxfId="1" priority="9">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I32">
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="0" priority="10">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="5">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="3" priority="6">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I32">
-    <cfRule type="expression" dxfId="2" priority="1">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
@@ -42207,18 +42154,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -42271,14 +42218,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -42288,6 +42227,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>